<commit_message>
Add new bug to README and updated test files
</commit_message>
<xml_diff>
--- a/docs/testing/jbtuition-automated-testing.xlsx
+++ b/docs/testing/jbtuition-automated-testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Development\Portfolio Projects\4. PP4 - John Breedon Tuition\README\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE817F7-AF8C-4179-8A23-C8EF699C2944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A664C73D-5605-453A-80AD-1D873555E7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bookings.forms.py" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
   <si>
     <t>John Breedon Bass Tuition Automated Testing</t>
   </si>
@@ -278,9 +278,6 @@
     <t>Test that the edit booking POST method updates the booking object</t>
   </si>
   <si>
-    <t>Test that the edit booking POST method prevents duplicate bookings</t>
-  </si>
-  <si>
     <t>Test that when user tries to POST an invalid booking to the edit view that the bookings page is re-rendered</t>
   </si>
   <si>
@@ -291,6 +288,12 @@
   </si>
   <si>
     <t>Test that the delete booking page GET method redirects if a user tries to delete another user's booking</t>
+  </si>
+  <si>
+    <t>Test that the edit booking POST method prevents booking onto a booked slot that is not the slot being edited</t>
+  </si>
+  <si>
+    <t>Tests that the edit booking POST method allows a user to edit just the lesson type on an existing booking</t>
   </si>
 </sst>
 </file>
@@ -629,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -723,10 +726,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF3526AE-45B2-46A3-B0F3-19852671E5B3}">
-  <dimension ref="B2:B24"/>
+  <dimension ref="B2:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,32 +809,37 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>